<commit_message>
1. multiple coluns in excel support added
</commit_message>
<xml_diff>
--- a/excel/Data-All.xlsx
+++ b/excel/Data-All.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="288" yWindow="456" windowWidth="22692" windowHeight="9144" activeTab="3"/>
+    <workbookView xWindow="288" yWindow="516" windowWidth="19872" windowHeight="8856" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="WebPlatforms_select" sheetId="3" r:id="rId1"/>
-    <sheet name="CR-create" sheetId="5" r:id="rId2"/>
+    <sheet name="CR-Create" sheetId="5" r:id="rId2"/>
     <sheet name="VA-Select-Delete" sheetId="2" r:id="rId3"/>
     <sheet name="VA-Create" sheetId="7" r:id="rId4"/>
   </sheets>
@@ -336,12 +336,6 @@
     <t xml:space="preserve">OAuthClientSecret </t>
   </si>
   <si>
-    <t xml:space="preserve">county    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">tag     </t>
-  </si>
-  <si>
     <t xml:space="preserve">moshe@gmail.com </t>
   </si>
   <si>
@@ -414,12 +408,6 @@
     <t>OAuthClientSecret-1</t>
   </si>
   <si>
-    <t>Israel</t>
-  </si>
-  <si>
-    <t>tag-1</t>
-  </si>
-  <si>
     <t>desc-2</t>
   </si>
   <si>
@@ -486,9 +474,6 @@
     <t>OAuthClientSecret-2</t>
   </si>
   <si>
-    <t>tag-2</t>
-  </si>
-  <si>
     <t>uName-2@gmail.com</t>
   </si>
   <si>
@@ -496,6 +481,21 @@
   </si>
   <si>
     <t>edit</t>
+  </si>
+  <si>
+    <t>0/5 * * * * ?</t>
+  </si>
+  <si>
+    <t>US##IL##UA</t>
+  </si>
+  <si>
+    <t>US-2##IL-2##UA-2</t>
+  </si>
+  <si>
+    <t>MOLOKO##man##drug</t>
+  </si>
+  <si>
+    <t>tag-2##tag-2</t>
   </si>
 </sst>
 </file>
@@ -1139,8 +1139,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1504,7 +1504,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection sqref="A1:B9"/>
     </sheetView>
   </sheetViews>
@@ -1600,8 +1600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1704,10 +1704,10 @@
         <v>79</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -1715,10 +1715,10 @@
         <v>80</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -1726,10 +1726,10 @@
         <v>81</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -1737,10 +1737,10 @@
         <v>82</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -1748,10 +1748,10 @@
         <v>83</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -1759,10 +1759,10 @@
         <v>84</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
@@ -1770,10 +1770,10 @@
         <v>85</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -1781,10 +1781,10 @@
         <v>86</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
@@ -1792,10 +1792,10 @@
         <v>87</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -1803,10 +1803,10 @@
         <v>88</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -1814,10 +1814,10 @@
         <v>89</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -1825,10 +1825,10 @@
         <v>90</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -1836,10 +1836,10 @@
         <v>91</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -1847,10 +1847,10 @@
         <v>92</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
@@ -1858,10 +1858,10 @@
         <v>93</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -1869,10 +1869,10 @@
         <v>94</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
@@ -1880,10 +1880,10 @@
         <v>95</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
@@ -1891,10 +1891,10 @@
         <v>96</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
@@ -1902,10 +1902,10 @@
         <v>97</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
@@ -1913,10 +1913,10 @@
         <v>98</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
@@ -1924,10 +1924,10 @@
         <v>99</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
@@ -1935,10 +1935,10 @@
         <v>100</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
@@ -1946,10 +1946,10 @@
         <v>101</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
@@ -1957,32 +1957,32 @@
         <v>102</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>103</v>
+        <v>42</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>129</v>
+        <v>153</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>129</v>
+        <v>154</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>130</v>
+      <c r="A34" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>155</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
@@ -1993,7 +1993,7 @@
         <v>22</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
@@ -2001,10 +2001,10 @@
         <v>51</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>69</v>
+        <v>152</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>